<commit_message>
Fix some bugs in virus sample export and import
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/virus_sample_import.xlsx
+++ b/baobab/lims/setupdata/test/virus_sample_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AnatomicalMaterial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Annuus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barcode</t>
   </si>
   <si>
     <t xml:space="preserve">Project</t>
@@ -378,7 +381,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -410,6 +413,22 @@
     <font>
       <b val="true"/>
       <sz val="11.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -472,7 +491,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -490,6 +509,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -497,7 +524,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,14 +547,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,8 +612,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,8 +671,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,8 +738,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,8 +813,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -848,9 +880,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -920,28 +953,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK5"/>
+  <dimension ref="A1:AL5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="30" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -987,10 +1024,10 @@
         <v>50</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>52</v>
@@ -1017,10 +1054,10 @@
         <v>59</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>61</v>
@@ -1049,19 +1086,23 @@
       <c r="AK1" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="0"/>
+        <v>71</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1080,10 +1121,10 @@
         <v>41</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>44</v>
@@ -1107,10 +1148,10 @@
         <v>50</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>52</v>
@@ -1137,10 +1178,10 @@
         <v>59</v>
       </c>
       <c r="AA3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="AC3" s="1" t="s">
         <v>61</v>
@@ -1169,30 +1210,33 @@
       <c r="AK3" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="AL3" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="G4" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>78</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -1201,14 +1245,14 @@
       <c r="L4" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="5" t="n">
+      <c r="M4" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="N4" s="7" t="n">
         <v>43031</v>
       </c>
-      <c r="N4" s="5" t="n">
+      <c r="O4" s="7" t="n">
         <v>44105</v>
-      </c>
-      <c r="O4" s="0" t="s">
-        <v>81</v>
       </c>
       <c r="P4" s="0" t="s">
         <v>82</v>
@@ -1232,31 +1276,31 @@
         <v>88</v>
       </c>
       <c r="W4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="X4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="Y4" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="Y4" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>90</v>
       </c>
       <c r="AA4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="AB4" s="0" t="s">
+      <c r="AC4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="AC4" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD4" s="0" t="n">
+      <c r="AD4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE4" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="AE4" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="AF4" s="0" t="s">
         <v>93</v>
@@ -1276,31 +1320,34 @@
       <c r="AK4" s="0" t="s">
         <v>98</v>
       </c>
+      <c r="AL4" s="0" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="D5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="F5" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="G5" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="J5" s="0" t="s">
         <v>102</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>103</v>
@@ -1308,71 +1355,74 @@
       <c r="L5" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="5" t="n">
+      <c r="M5" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="7" t="n">
         <v>44158</v>
       </c>
-      <c r="N5" s="5" t="n">
+      <c r="O5" s="7" t="n">
         <v>44166</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>105</v>
       </c>
       <c r="P5" s="0" t="s">
         <v>106</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="S5" s="0" t="s">
         <v>108</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="U5" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="W5" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="V5" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="Z5" s="0" t="s">
-        <v>110</v>
-      </c>
       <c r="AA5" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="AB5" s="0" t="s">
+      <c r="AC5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="AD5" s="0" t="n">
+      <c r="AD5" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AE5" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="AE5" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="AF5" s="0" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="AG5" s="0" t="s">
         <v>94</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="AJ5" s="0" t="s">
         <v>97</v>
       </c>
       <c r="AK5" s="0" t="s">
-        <v>113</v>
+        <v>98</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separate Biospecimen from Virus Sample and fix the importer
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/virus_sample_import.xlsx
+++ b/baobab/lims/setupdata/test/virus_sample_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AnatomicalMaterial" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="118">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -154,60 +154,66 @@
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
+    <t xml:space="preserve">Anatomical Site Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anatomical Site Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allow Sharing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WillReturnFromShipment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BioSampleAccession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecimenCollectorSampleID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleCollectedBy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleCollectionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SampleReceivedDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoLocCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GeoLocState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isolate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PurposeOfSampling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CollectionDevice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CollectionProtocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecimenProcessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LabHost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PassageNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PassageMethod</t>
+  </si>
+  <si>
     <t xml:space="preserve">AnatomicalMaterial</t>
   </si>
   <si>
-    <t xml:space="preserve">Allow Sharing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WillReturnFromShipment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BioSampleAccession</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpecimenCollectorSampleID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SampleCollectedBy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SampleCollectionDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SampleReceivedDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoLocCountry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GeoLocState</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isolate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PurposeOfSampling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CollectionDevice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CollectionProtocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SpecimenProcessing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LabHost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PassageNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PassageMethod</t>
-  </si>
-  <si>
     <t xml:space="preserve">HostSubjectID</t>
   </si>
   <si>
@@ -241,13 +247,16 @@
     <t xml:space="preserve">SequencingProtocolName</t>
   </si>
   <si>
-    <t xml:space="preserve">Virus Sample</t>
+    <t xml:space="preserve">AnatomicalSiteTerm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnatomicalSiteDescription</t>
   </si>
   <si>
     <t xml:space="preserve">AllowSharing</t>
   </si>
   <si>
-    <t xml:space="preserve">E4011</t>
+    <t xml:space="preserve">E4016</t>
   </si>
   <si>
     <t xml:space="preserve">Green Goblin Project</t>
@@ -262,45 +271,45 @@
     <t xml:space="preserve">ml</t>
   </si>
   <si>
+    <t xml:space="preserve">A1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Cameron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canberra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tresae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extraction Device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protocol X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virus Passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The method of doing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Arm</t>
   </si>
   <si>
-    <t xml:space="preserve">A1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Cameron</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Australia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canberra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rocket</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tresae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extraction Device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">protocol X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virus Passage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The method of doing</t>
-  </si>
-  <si>
     <t xml:space="preserve">H10021</t>
   </si>
   <si>
@@ -328,7 +337,7 @@
     <t xml:space="preserve">Protocol Z</t>
   </si>
   <si>
-    <t xml:space="preserve">E4013</t>
+    <t xml:space="preserve">E4015</t>
   </si>
   <si>
     <t xml:space="preserve">Room-2.Freezer-1.Box-01.17</t>
@@ -553,9 +562,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,9 +621,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.8622448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -671,9 +680,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="70.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -738,9 +747,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,9 +822,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -880,10 +889,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,300 +962,305 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AL5"/>
+  <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="30" min="16" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.1989795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="28.3367346938776"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.8622448979592"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.1938775510204"/>
+    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="0"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="0"/>
-    </row>
-    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AC3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AD3" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="G4" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>78</v>
+      <c r="F4" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="N4" s="7" t="n">
         <v>43031</v>
@@ -1255,28 +1269,28 @@
         <v>44105</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="X4" s="0" t="s">
         <v>21</v>
@@ -1285,78 +1299,75 @@
         <v>2</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="AB4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="AC4" s="0" t="s">
+      <c r="AD4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE4" s="0" t="n">
+      <c r="AE4" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="AF4" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="AG4" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AI4" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="AJ4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AK4" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AL4" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>78</v>
+      <c r="F5" s="0" t="s">
+        <v>105</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="N5" s="7" t="n">
         <v>44158</v>
@@ -1365,64 +1376,67 @@
         <v>44166</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="AB5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="AC5" s="0" t="s">
+      <c r="AD5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="AD5" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE5" s="0" t="n">
+      <c r="AE5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF5" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="AF5" s="0" t="s">
-        <v>112</v>
-      </c>
       <c r="AG5" s="0" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AI5" s="0" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="AK5" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AL5" s="0" t="s">
-        <v>114</v>
+        <v>101</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix virus samples for use in viral genomic analysis
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/virus_sample_import.xlsx
+++ b/baobab/lims/setupdata/test/virus_sample_import.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AnatomicalMaterial" sheetId="1" state="visible" r:id="rId2"/>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">AllowSharing</t>
   </si>
   <si>
-    <t xml:space="preserve">E4016</t>
+    <t xml:space="preserve">E4017</t>
   </si>
   <si>
     <t xml:space="preserve">Green Goblin Project</t>
@@ -337,7 +337,7 @@
     <t xml:space="preserve">Protocol Z</t>
   </si>
   <si>
-    <t xml:space="preserve">E4015</t>
+    <t xml:space="preserve">E4018</t>
   </si>
   <si>
     <t xml:space="preserve">Room-2.Freezer-1.Box-01.17</t>
@@ -562,9 +562,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,9 +621,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,9 +680,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,9 +747,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.1224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,9 +822,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,10 +889,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,28 +965,28 @@
   <dimension ref="1:5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.1989795918367"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="28.3367346938776"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.8622448979592"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.1938775510204"/>
-    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="27.9438775510204"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Changes to the importer
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/virus_sample_import.xlsx
+++ b/baobab/lims/setupdata/test/virus_sample_import.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -380,6 +380,15 @@
   </si>
   <si>
     <t xml:space="preserve">Protocol Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LFA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4020</t>
   </si>
 </sst>
 </file>
@@ -562,9 +571,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.8622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5408163265306"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,9 +629,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -680,9 +687,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.9795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.1683673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -747,9 +753,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,9 +827,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,10 +893,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -962,31 +965,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5"/>
+  <dimension ref="1:7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.6530612244898"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1436,6 +1434,211 @@
         <v>101</v>
       </c>
       <c r="AM5" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="7" t="n">
+        <v>43031</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>44105</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="U6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE6" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="7" t="n">
+        <v>44158</v>
+      </c>
+      <c r="O7" s="7" t="n">
+        <v>44166</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="T7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="U7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF7" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL7" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM7" s="0" t="s">
         <v>117</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix importer for samples as well as virus samples
</commit_message>
<xml_diff>
--- a/baobab/lims/setupdata/test/virus_sample_import.xlsx
+++ b/baobab/lims/setupdata/test/virus_sample_import.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="126">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">AllowSharing</t>
   </si>
   <si>
-    <t xml:space="preserve">E4017</t>
+    <t xml:space="preserve">E4055</t>
   </si>
   <si>
     <t xml:space="preserve">Green Goblin Project</t>
@@ -265,7 +265,7 @@
     <t xml:space="preserve">Whole Blood</t>
   </si>
   <si>
-    <t xml:space="preserve">Room-2.Freezer-1.Box-01.10</t>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.20</t>
   </si>
   <si>
     <t xml:space="preserve">ml</t>
@@ -337,7 +337,10 @@
     <t xml:space="preserve">Protocol Z</t>
   </si>
   <si>
-    <t xml:space="preserve">E4018</t>
+    <t xml:space="preserve">E4041</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LFA</t>
   </si>
   <si>
     <t xml:space="preserve">Room-2.Freezer-1.Box-01.17</t>
@@ -385,10 +388,22 @@
     <t xml:space="preserve">E4019</t>
   </si>
   <si>
-    <t xml:space="preserve">LFA</t>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.15</t>
   </si>
   <si>
     <t xml:space="preserve">E4020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E4042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Room-2.Freezer-1.Box-01.24</t>
   </si>
 </sst>
 </file>
@@ -571,8 +586,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -629,8 +645,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.4336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,8 +704,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="68.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -753,8 +771,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -827,8 +846,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1632653061224"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -893,9 +913,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -965,26 +986,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:7"/>
+  <dimension ref="1:9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="27.6734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.0663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="25" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="31" min="28" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="34" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,28 +1371,28 @@
         <v>103</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>24</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N5" s="7" t="n">
         <v>44158</v>
@@ -1374,34 +1401,34 @@
         <v>44166</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>86</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U5" s="0" t="s">
         <v>93</v>
       </c>
       <c r="V5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="W5" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="W5" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="AA5" s="0" t="s">
         <v>93</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AC5" s="0" t="s">
         <v>9</v>
@@ -1416,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="AG5" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AH5" s="0" t="s">
         <v>97</v>
@@ -1425,7 +1452,7 @@
         <v>98</v>
       </c>
       <c r="AJ5" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AK5" s="0" t="s">
         <v>100</v>
@@ -1434,21 +1461,21 @@
         <v>101</v>
       </c>
       <c r="AM5" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>79</v>
+        <v>120</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>12</v>
@@ -1546,31 +1573,31 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>24</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N7" s="7" t="n">
         <v>44158</v>
@@ -1579,34 +1606,34 @@
         <v>44166</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="R7" s="0" t="s">
         <v>86</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="U7" s="0" t="s">
         <v>93</v>
       </c>
       <c r="V7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>112</v>
       </c>
       <c r="AA7" s="0" t="s">
         <v>93</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AC7" s="0" t="s">
         <v>9</v>
@@ -1621,7 +1648,7 @@
         <v>18</v>
       </c>
       <c r="AG7" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AH7" s="0" t="s">
         <v>97</v>
@@ -1630,7 +1657,7 @@
         <v>98</v>
       </c>
       <c r="AJ7" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AK7" s="0" t="s">
         <v>100</v>
@@ -1639,7 +1666,221 @@
         <v>101</v>
       </c>
       <c r="AM7" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8" s="7" t="n">
+        <v>43031</v>
+      </c>
+      <c r="O8" s="7" t="n">
+        <v>44105</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="V8" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="W8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB8" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="N9" s="7" t="n">
+        <v>43031</v>
+      </c>
+      <c r="O9" s="7" t="n">
+        <v>44105</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="S9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="T9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="U9" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="V9" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="W9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA9" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB9" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AF9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI9" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AJ9" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL9" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="AM9" s="0" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>